<commit_message>
finish check statment with date, empty rows fix
</commit_message>
<xml_diff>
--- a/test files/Biblio- Siva.xlsx
+++ b/test files/Biblio- Siva.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vscoded\Credit_App\Credit_App\test files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E005AD4D-0C1C-4931-95BC-8591F0B2DFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="statment" sheetId="6" r:id="rId1"/>
@@ -23,7 +17,7 @@
     <sheet name="spo 24.11 only" sheetId="13" r:id="rId8"/>
     <sheet name="spo 25.11 to 15.02.24" sheetId="14" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -155,11 +149,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;_-* #,##0.00\-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="d/mm/yyyy;@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;_-* #,##0.00\-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -556,7 +551,7 @@
   </borders>
   <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
@@ -597,7 +592,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -674,19 +669,19 @@
     <xf numFmtId="1" fontId="5" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="6" fillId="9" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -698,20 +693,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="6" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="6" fillId="9" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -785,54 +780,57 @@
     <xf numFmtId="0" fontId="13" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="5" fillId="9" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="11" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="11" fillId="9" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="5" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="5" fillId="9" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="11" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="11" fillId="9" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="5" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="5" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="41">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 10 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 10 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 140" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 148" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 149" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 151" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 152" xfId="40" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 153" xfId="9" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 154" xfId="10" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Normal 157" xfId="38" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Normal 158" xfId="39" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Normal 159" xfId="11" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Normal 160" xfId="12" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Normal 162" xfId="13" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Normal 163" xfId="14" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Normal 165" xfId="15" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Normal 166" xfId="16" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Normal 19 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Normal 19 3" xfId="18" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Normal 19 4" xfId="19" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Normal 2 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Normal 2 3" xfId="21" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Normal 2 4" xfId="22" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Normal 20 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Normal 20 3" xfId="24" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Normal 20 4" xfId="25" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Normal 23 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Normal 23 3" xfId="27" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Normal 23 4" xfId="28" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Normal 37 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Normal 37 3" xfId="30" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Normal 37 4" xfId="31" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Normal 38 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Normal 38 3" xfId="33" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Normal 38 4" xfId="34" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Normal 9 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Normal 9 3" xfId="36" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Normal 9 4" xfId="37" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 10 2" xfId="2"/>
+    <cellStyle name="Normal 10 3" xfId="3"/>
+    <cellStyle name="Normal 10 4" xfId="4"/>
+    <cellStyle name="Normal 140" xfId="5"/>
+    <cellStyle name="Normal 148" xfId="6"/>
+    <cellStyle name="Normal 149" xfId="7"/>
+    <cellStyle name="Normal 151" xfId="8"/>
+    <cellStyle name="Normal 152" xfId="40"/>
+    <cellStyle name="Normal 153" xfId="9"/>
+    <cellStyle name="Normal 154" xfId="10"/>
+    <cellStyle name="Normal 157" xfId="38"/>
+    <cellStyle name="Normal 158" xfId="39"/>
+    <cellStyle name="Normal 159" xfId="11"/>
+    <cellStyle name="Normal 160" xfId="12"/>
+    <cellStyle name="Normal 162" xfId="13"/>
+    <cellStyle name="Normal 163" xfId="14"/>
+    <cellStyle name="Normal 165" xfId="15"/>
+    <cellStyle name="Normal 166" xfId="16"/>
+    <cellStyle name="Normal 19 2" xfId="17"/>
+    <cellStyle name="Normal 19 3" xfId="18"/>
+    <cellStyle name="Normal 19 4" xfId="19"/>
+    <cellStyle name="Normal 2 2" xfId="20"/>
+    <cellStyle name="Normal 2 3" xfId="21"/>
+    <cellStyle name="Normal 2 4" xfId="22"/>
+    <cellStyle name="Normal 20 2" xfId="23"/>
+    <cellStyle name="Normal 20 3" xfId="24"/>
+    <cellStyle name="Normal 20 4" xfId="25"/>
+    <cellStyle name="Normal 23 2" xfId="26"/>
+    <cellStyle name="Normal 23 3" xfId="27"/>
+    <cellStyle name="Normal 23 4" xfId="28"/>
+    <cellStyle name="Normal 37 2" xfId="29"/>
+    <cellStyle name="Normal 37 3" xfId="30"/>
+    <cellStyle name="Normal 37 4" xfId="31"/>
+    <cellStyle name="Normal 38 2" xfId="32"/>
+    <cellStyle name="Normal 38 3" xfId="33"/>
+    <cellStyle name="Normal 38 4" xfId="34"/>
+    <cellStyle name="Normal 9 2" xfId="35"/>
+    <cellStyle name="Normal 9 3" xfId="36"/>
+    <cellStyle name="Normal 9 4" xfId="37"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -890,7 +888,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -922,27 +920,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -974,24 +954,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1167,26 +1129,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="15" width="20.6640625" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="15" width="20.7109375" customWidth="1"/>
     <col min="16" max="16" width="25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.6640625" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.600000000000001" thickTop="1" thickBot="1">
+    <row r="1" spans="1:17" ht="20.25" thickTop="1" thickBot="1">
       <c r="B1" s="13" t="s">
         <v>18</v>
       </c>
@@ -1236,7 +1198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.6" thickTop="1">
+    <row r="2" spans="1:17" ht="15.75" thickTop="1">
       <c r="A2" s="15"/>
       <c r="B2" s="16">
         <v>1</v>
@@ -1252,7 +1214,7 @@
       </c>
       <c r="F2" s="29"/>
       <c r="G2" s="30"/>
-      <c r="H2" s="31">
+      <c r="H2" s="72">
         <v>45230</v>
       </c>
       <c r="I2" s="31">
@@ -2693,21 +2655,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.4" thickTop="1">
+    <row r="1" spans="1:14" ht="15.75" thickTop="1">
       <c r="A1" s="58" t="s">
         <v>9</v>
       </c>
@@ -2751,7 +2713,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="13.8">
+    <row r="2" spans="1:14" ht="14.25">
       <c r="A2" s="52">
         <v>45047</v>
       </c>
@@ -2795,7 +2757,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="13.8">
+    <row r="3" spans="1:14" ht="14.25">
       <c r="A3" s="52">
         <v>45062</v>
       </c>
@@ -2839,7 +2801,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="13.8">
+    <row r="4" spans="1:14" ht="14.25">
       <c r="A4" s="52">
         <v>45078</v>
       </c>
@@ -2883,7 +2845,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="13.8">
+    <row r="5" spans="1:14" ht="14.25">
       <c r="A5" s="52">
         <v>45108</v>
       </c>
@@ -2927,7 +2889,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="13.8">
+    <row r="6" spans="1:14" ht="14.25">
       <c r="A6" s="52">
         <v>45139</v>
       </c>
@@ -2971,7 +2933,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="13.8">
+    <row r="7" spans="1:14" ht="14.25">
       <c r="A7" s="52">
         <v>45170</v>
       </c>
@@ -3015,7 +2977,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="13.8">
+    <row r="8" spans="1:14" ht="14.25">
       <c r="A8" s="52">
         <v>45200</v>
       </c>
@@ -3059,7 +3021,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="13.8">
+    <row r="9" spans="1:14" ht="14.25">
       <c r="A9" s="52">
         <v>45231</v>
       </c>
@@ -3109,7 +3071,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="13.8">
+    <row r="10" spans="1:14" ht="14.25">
       <c r="A10" s="52">
         <v>45246</v>
       </c>
@@ -3159,7 +3121,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="13.8">
+    <row r="11" spans="1:14" ht="14.25">
       <c r="A11" s="52">
         <v>45289</v>
       </c>
@@ -3209,7 +3171,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="13.8">
+    <row r="12" spans="1:14" ht="14.25">
       <c r="A12" s="52">
         <v>45302</v>
       </c>
@@ -3259,7 +3221,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="14.4" thickBot="1">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="55">
         <v>45338</v>
       </c>
@@ -3309,7 +3271,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="13.8" thickTop="1"/>
+    <row r="14" spans="1:14" ht="13.5" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3317,22 +3279,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="14.4" thickBot="1">
+    <row r="1" spans="1:15" ht="15" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -3379,7 +3341,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="14.4" thickTop="1">
+    <row r="2" spans="1:15" ht="15" thickTop="1">
       <c r="A2" s="6">
         <v>45119</v>
       </c>
@@ -3427,7 +3389,7 @@
         <v>102.5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="13.8">
+    <row r="3" spans="1:15" ht="14.25">
       <c r="A3" s="9">
         <v>45139</v>
       </c>
@@ -3475,7 +3437,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="13.8">
+    <row r="4" spans="1:15" ht="14.25">
       <c r="A4" s="9">
         <v>45170</v>
       </c>
@@ -3529,22 +3491,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="13.8">
+    <row r="1" spans="1:15" ht="14.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -3591,7 +3553,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="13.8">
+    <row r="2" spans="1:15" ht="14.25">
       <c r="A2" s="9">
         <v>45139</v>
       </c>
@@ -3645,21 +3607,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.4" thickTop="1">
+    <row r="1" spans="1:13" ht="15.75" thickTop="1">
       <c r="A1" s="58" t="s">
         <v>9</v>
       </c>
@@ -3700,7 +3662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.8">
+    <row r="2" spans="1:13" ht="14.25">
       <c r="A2" s="52">
         <v>45228</v>
       </c>
@@ -3749,7 +3711,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="13.8">
+    <row r="3" spans="1:13" ht="14.25">
       <c r="A3" s="52">
         <v>45289</v>
       </c>
@@ -3798,7 +3760,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="13.8">
+    <row r="4" spans="1:13" ht="14.25">
       <c r="A4" s="52">
         <v>45296</v>
       </c>
@@ -3854,21 +3816,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.4" thickTop="1">
+    <row r="1" spans="1:13" ht="15.75" thickTop="1">
       <c r="A1" s="58" t="s">
         <v>9</v>
       </c>
@@ -3909,7 +3871,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.8">
+    <row r="2" spans="1:13" ht="14.25">
       <c r="A2" s="52">
         <v>45234</v>
       </c>
@@ -3958,7 +3920,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="13.8">
+    <row r="3" spans="1:13" ht="14.25">
       <c r="A3" s="52">
         <v>45289</v>
       </c>
@@ -4007,7 +3969,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="13.8">
+    <row r="4" spans="1:13" ht="14.25">
       <c r="A4" s="52">
         <v>45296</v>
       </c>
@@ -4063,21 +4025,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.4" thickTop="1">
+    <row r="1" spans="1:13" ht="15.75" thickTop="1">
       <c r="A1" s="58" t="s">
         <v>9</v>
       </c>
@@ -4118,7 +4080,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.8">
+    <row r="2" spans="1:13" ht="14.25">
       <c r="A2" s="52">
         <v>45247</v>
       </c>
@@ -4167,7 +4129,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="13.8">
+    <row r="3" spans="1:13" ht="14.25">
       <c r="A3" s="52">
         <v>45289</v>
       </c>
@@ -4216,7 +4178,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="13.8">
+    <row r="4" spans="1:13" ht="14.25">
       <c r="A4" s="52">
         <v>45296</v>
       </c>
@@ -4272,22 +4234,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.4" thickTop="1">
+    <row r="1" spans="1:13" ht="15.75" thickTop="1">
       <c r="A1" s="58" t="s">
         <v>9</v>
       </c>
@@ -4328,7 +4290,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.8">
+    <row r="2" spans="1:13" ht="14.25">
       <c r="A2" s="52">
         <v>45254</v>
       </c>
@@ -4377,7 +4339,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="13.8">
+    <row r="3" spans="1:13" ht="14.25">
       <c r="A3" s="52">
         <v>45289</v>
       </c>
@@ -4426,7 +4388,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="13.8">
+    <row r="4" spans="1:13" ht="14.25">
       <c r="A4" s="52">
         <v>45296</v>
       </c>
@@ -4475,7 +4437,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="13.8">
+    <row r="5" spans="1:13" ht="14.25">
       <c r="A5" s="52">
         <v>45338</v>
       </c>
@@ -4531,21 +4493,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.4" thickTop="1">
+    <row r="1" spans="1:13" ht="15.75" thickTop="1">
       <c r="A1" s="58" t="s">
         <v>9</v>
       </c>
@@ -4586,7 +4548,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.8">
+    <row r="2" spans="1:13" ht="14.25">
       <c r="A2" s="52">
         <v>45247</v>
       </c>
@@ -4635,7 +4597,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="13.8">
+    <row r="3" spans="1:13" ht="14.25">
       <c r="A3" s="52">
         <v>45289</v>
       </c>
@@ -4684,7 +4646,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="13.8">
+    <row r="4" spans="1:13" ht="14.25">
       <c r="A4" s="52">
         <v>45296</v>
       </c>

</xml_diff>

<commit_message>
make app with browse in homepage and add toggle menu
</commit_message>
<xml_diff>
--- a/test files/Biblio- Siva.xlsx
+++ b/test files/Biblio- Siva.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="statment" sheetId="6" r:id="rId1"/>
@@ -3282,7 +3282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4237,8 +4237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4290,7 +4290,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.25">
+    <row r="2" spans="1:13" ht="12.75" customHeight="1">
       <c r="A2" s="52">
         <v>45254</v>
       </c>
@@ -4390,7 +4390,7 @@
     </row>
     <row r="4" spans="1:13" ht="14.25">
       <c r="A4" s="52">
-        <v>45296</v>
+        <v>45327</v>
       </c>
       <c r="B4" s="52">
         <v>45337</v>

</xml_diff>